<commit_message>
finishing first line graph
</commit_message>
<xml_diff>
--- a/Original Plot Work/1906 - 1913 Tuberculosis Mortality Country&Town/Tuberculosis Towns.xlsx
+++ b/Original Plot Work/1906 - 1913 Tuberculosis Mortality Country&Town/Tuberculosis Towns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RBY11\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9797368-9261-473B-93B7-E1FA8C2C971B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CFD71F-9C21-467C-B368-90F90DA712E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11925" yWindow="4095" windowWidth="21600" windowHeight="11835" xr2:uid="{96BF90FF-1741-4FBC-A155-E4DE914473FC}"/>
+    <workbookView xWindow="2355" yWindow="3615" windowWidth="21600" windowHeight="11835" xr2:uid="{96BF90FF-1741-4FBC-A155-E4DE914473FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="8">
   <si>
     <t>Year</t>
   </si>
@@ -57,15 +57,24 @@
   <si>
     <t>Rural France</t>
   </si>
+  <si>
+    <t>TFrench Cities</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -407,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54913F4-3402-4593-AAB7-E2938A1C8BA2}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,7 +726,7 @@
         <v>1908</v>
       </c>
       <c r="B28">
-        <v>1.82</v>
+        <v>1.62</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -778,7 +787,96 @@
         <v>6</v>
       </c>
     </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1906</v>
+      </c>
+      <c r="B34">
+        <v>3.25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1907</v>
+      </c>
+      <c r="B35">
+        <v>3.32</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1908</v>
+      </c>
+      <c r="B36">
+        <v>3.25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1909</v>
+      </c>
+      <c r="B37">
+        <v>3.13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1910</v>
+      </c>
+      <c r="B38">
+        <v>3.14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1911</v>
+      </c>
+      <c r="B39">
+        <v>3.15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1912</v>
+      </c>
+      <c r="B40">
+        <v>3.03</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1913</v>
+      </c>
+      <c r="B41">
+        <v>3.07</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>